<commit_message>
face stat salarii, nu complet -> vezi todo
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Septembrie 2020.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Ingenio Software S.A. - Septembrie 2020.xlsx
@@ -2090,7 +2090,7 @@
         <v>0.0</v>
       </c>
       <c r="O21" s="53" t="n">
-        <v>220.0</v>
+        <v>0.0</v>
       </c>
       <c r="P21" s="53" t="n">
         <v>0.0</v>
@@ -2102,7 +2102,7 @@
         <v>0.0</v>
       </c>
       <c r="S21" s="53" t="n">
-        <v>152.0</v>
+        <v>130.0</v>
       </c>
       <c r="T21" s="53" t="n">
         <v>0.0</v>
@@ -2154,10 +2154,10 @@
         <v>251.0</v>
       </c>
       <c r="R22" s="40" t="n">
-        <v>1478.0</v>
+        <v>1500.0</v>
       </c>
       <c r="S22" t="n" s="40">
-        <v>1478.0</v>
+        <v>1500.0</v>
       </c>
       <c r="T22" s="40" t="n">
         <v>0.0</v>
@@ -2215,7 +2215,7 @@
         <v>0.0</v>
       </c>
       <c r="T23" s="46" t="n">
-        <v>1478.0</v>
+        <v>1500.0</v>
       </c>
       <c r="U23" s="50"/>
     </row>
@@ -2248,10 +2248,10 @@
         <v>160.0</v>
       </c>
       <c r="L24" s="53" t="n">
-        <v>5454.0</v>
+        <v>4958.0</v>
       </c>
       <c r="M24" s="53" t="n">
-        <v>0.0</v>
+        <v>498.0</v>
       </c>
       <c r="N24" s="53" t="n">
         <v>0.0</v>
@@ -2312,13 +2312,13 @@
         <v>0.0</v>
       </c>
       <c r="O25" s="40" t="n">
-        <v>5454.0</v>
+        <v>5456.0</v>
       </c>
       <c r="P25" s="40" t="n">
         <v>0.0</v>
       </c>
       <c r="Q25" s="40" t="n">
-        <v>545.0</v>
+        <v>546.0</v>
       </c>
       <c r="R25" s="40" t="n">
         <v>3191.0</v>

</xml_diff>